<commit_message>
lista de tablas & renombrar tabla resumen
</commit_message>
<xml_diff>
--- a/Lista_programas_inputs_outputs.xlsx
+++ b/Lista_programas_inputs_outputs.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\7. Work\covid_cusco\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\GitHub\covid_cusco\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25A49533-4270-406C-B8A4-C1537F908D1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4672C4BA-47B3-4A0F-9B38-2E56F485772C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2820" windowWidth="23040" windowHeight="7320" xr2:uid="{6F1C67DC-F352-4C08-898E-8C30B2794AD3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6F1C67DC-F352-4C08-898E-8C30B2794AD3}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Hoja1!$A$1:$E$130</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Hoja1!$A$1:$E$139</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="270">
   <si>
     <t>Programa</t>
   </si>
@@ -849,6 +849,24 @@
   </si>
   <si>
     <t>mortalidad_provincial_2021.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tablas </t>
+  </si>
+  <si>
+    <t>tabla_positividad_provincia.tex</t>
+  </si>
+  <si>
+    <t>tabla_incidencia_provincia.tex</t>
+  </si>
+  <si>
+    <t>tabla_letalidad_mortalidad_provincia.tex</t>
+  </si>
+  <si>
+    <t>tabla_resumen.tex</t>
+  </si>
+  <si>
+    <t>tabla_defunciones_cero_provincia.tex</t>
   </si>
 </sst>
 </file>
@@ -1294,10 +1312,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:XFD130"/>
+  <dimension ref="A1:XFD138"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A106" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A129" sqref="A129"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A98" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B132" sqref="B132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2119,25 +2137,25 @@
         <v>127</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A84" s="7"/>
-      <c r="B84" s="7"/>
-      <c r="C84" s="7" t="s">
+    <row r="84" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="13"/>
+      <c r="B84" s="13"/>
+      <c r="C84" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="D84" s="7" t="s">
+      <c r="D84" s="13" t="s">
         <v>129</v>
       </c>
       <c r="E84" s="13"/>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A85" s="7"/>
       <c r="B85" s="7"/>
       <c r="C85" s="7"/>
       <c r="D85" s="7"/>
       <c r="E85" s="7"/>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A86" s="6" t="s">
         <v>150</v>
       </c>
@@ -2146,7 +2164,7 @@
       <c r="D86" s="7"/>
       <c r="E86" s="7"/>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>151</v>
       </c>
@@ -2160,37 +2178,37 @@
         <v>224</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B88" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B89" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B90" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B91" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B92" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B93" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>152</v>
       </c>
@@ -2204,7 +2222,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>153</v>
       </c>
@@ -2215,12 +2233,12 @@
         <v>226</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B96" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>154</v>
       </c>
@@ -2237,7 +2255,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>155</v>
       </c>
@@ -2254,7 +2272,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B99" t="s">
         <v>167</v>
       </c>
@@ -2265,7 +2283,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B100" t="s">
         <v>168</v>
       </c>
@@ -2276,7 +2294,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B101" t="s">
         <v>168</v>
       </c>
@@ -2287,7 +2305,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B102" t="s">
         <v>169</v>
       </c>
@@ -2298,7 +2316,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B103" t="s">
         <v>170</v>
       </c>
@@ -2309,12 +2327,12 @@
         <v>183</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B104" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A105" s="13"/>
       <c r="B105" s="13" t="s">
         <v>171</v>
@@ -2323,14 +2341,14 @@
       <c r="D105" s="13"/>
       <c r="E105" s="13"/>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A106" s="7"/>
       <c r="B106" s="7"/>
       <c r="C106" s="7"/>
       <c r="D106" s="7"/>
       <c r="E106" s="7"/>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A107" s="6" t="s">
         <v>249</v>
       </c>
@@ -2339,7 +2357,7 @@
       <c r="D107" s="7"/>
       <c r="E107" s="7"/>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>147</v>
       </c>
@@ -2350,7 +2368,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>186</v>
       </c>
@@ -2367,7 +2385,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B110" t="s">
         <v>149</v>
       </c>
@@ -2375,7 +2393,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B111" t="s">
         <v>6</v>
       </c>
@@ -2386,14 +2404,14 @@
         <v>191</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A112" s="7"/>
       <c r="B112" s="7"/>
       <c r="C112" s="7"/>
       <c r="D112" s="7"/>
       <c r="E112" s="7"/>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A113" s="14" t="s">
         <v>137</v>
       </c>
@@ -2402,7 +2420,7 @@
       <c r="D113" s="7"/>
       <c r="E113" s="7"/>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>237</v>
       </c>
@@ -2416,7 +2434,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>238</v>
       </c>
@@ -2427,7 +2445,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>239</v>
       </c>
@@ -2441,7 +2459,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B117" t="s">
         <v>144</v>
       </c>
@@ -2449,12 +2467,12 @@
         <v>232</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B118" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>240</v>
       </c>
@@ -2468,17 +2486,17 @@
         <v>233</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B120" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B121" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A122" s="3" t="s">
         <v>234</v>
       </c>
@@ -2492,7 +2510,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C123" t="s">
         <v>253</v>
       </c>
@@ -2500,12 +2518,12 @@
         <v>254</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C124" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C125" t="s">
         <v>255</v>
       </c>
@@ -2513,12 +2531,12 @@
         <v>256</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C126" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C127" t="s">
         <v>257</v>
       </c>
@@ -2566,6 +2584,40 @@
       </c>
       <c r="D130" t="s">
         <v>263</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="132" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A132" s="7"/>
+    </row>
+    <row r="133" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A133" s="6" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A134" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A135" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A136" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A137" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A138" t="s">
+        <v>269</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tabla de. cero setting
</commit_message>
<xml_diff>
--- a/Lista_programas_inputs_outputs.xlsx
+++ b/Lista_programas_inputs_outputs.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\GitHub\covid_cusco\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4672C4BA-47B3-4A0F-9B38-2E56F485772C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F2957CC-41AF-47FF-BA2D-C30F9AB56DAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6F1C67DC-F352-4C08-898E-8C30B2794AD3}"/>
+    <workbookView xWindow="-13704" yWindow="8448" windowWidth="23040" windowHeight="7320" xr2:uid="{6F1C67DC-F352-4C08-898E-8C30B2794AD3}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Hoja1!$A$1:$E$139</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Hoja1!$A$1:$E$140</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="271">
   <si>
     <t>Programa</t>
   </si>
@@ -867,6 +867,9 @@
   </si>
   <si>
     <t>tabla_defunciones_cero_provincia.tex</t>
+  </si>
+  <si>
+    <t>4z_tabla_cero_defunciones.do</t>
   </si>
 </sst>
 </file>
@@ -1314,8 +1317,8 @@
   </sheetPr>
   <dimension ref="A1:XFD138"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A98" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B132" sqref="B132"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A108" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D137" sqref="D137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2137,7 +2140,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="84" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" s="13"/>
       <c r="B84" s="13"/>
       <c r="C84" s="13" t="s">
@@ -2148,14 +2151,14 @@
       </c>
       <c r="E84" s="13"/>
     </row>
-    <row r="85" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" s="7"/>
       <c r="B85" s="7"/>
       <c r="C85" s="7"/>
       <c r="D85" s="7"/>
       <c r="E85" s="7"/>
     </row>
-    <row r="86" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" s="6" t="s">
         <v>150</v>
       </c>
@@ -2164,7 +2167,7 @@
       <c r="D86" s="7"/>
       <c r="E86" s="7"/>
     </row>
-    <row r="87" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>151</v>
       </c>
@@ -2178,37 +2181,37 @@
         <v>224</v>
       </c>
     </row>
-    <row r="88" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B88" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="89" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B89" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="90" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B90" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="91" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B91" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="92" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B92" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="93" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B93" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="94" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>152</v>
       </c>
@@ -2222,7 +2225,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="95" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>153</v>
       </c>
@@ -2233,12 +2236,12 @@
         <v>226</v>
       </c>
     </row>
-    <row r="96" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B96" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="97" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>154</v>
       </c>
@@ -2255,7 +2258,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="98" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>155</v>
       </c>
@@ -2272,7 +2275,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="99" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B99" t="s">
         <v>167</v>
       </c>
@@ -2283,7 +2286,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="100" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B100" t="s">
         <v>168</v>
       </c>
@@ -2294,7 +2297,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="101" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B101" t="s">
         <v>168</v>
       </c>
@@ -2305,7 +2308,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="102" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B102" t="s">
         <v>169</v>
       </c>
@@ -2316,7 +2319,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="103" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B103" t="s">
         <v>170</v>
       </c>
@@ -2327,12 +2330,12 @@
         <v>183</v>
       </c>
     </row>
-    <row r="104" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B104" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="105" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" s="13"/>
       <c r="B105" s="13" t="s">
         <v>171</v>
@@ -2341,14 +2344,14 @@
       <c r="D105" s="13"/>
       <c r="E105" s="13"/>
     </row>
-    <row r="106" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" s="7"/>
       <c r="B106" s="7"/>
       <c r="C106" s="7"/>
       <c r="D106" s="7"/>
       <c r="E106" s="7"/>
     </row>
-    <row r="107" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" s="6" t="s">
         <v>249</v>
       </c>
@@ -2357,7 +2360,7 @@
       <c r="D107" s="7"/>
       <c r="E107" s="7"/>
     </row>
-    <row r="108" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>147</v>
       </c>
@@ -2368,7 +2371,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="109" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>186</v>
       </c>
@@ -2385,7 +2388,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="110" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B110" t="s">
         <v>149</v>
       </c>
@@ -2393,7 +2396,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="111" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B111" t="s">
         <v>6</v>
       </c>
@@ -2404,14 +2407,14 @@
         <v>191</v>
       </c>
     </row>
-    <row r="112" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112" s="7"/>
       <c r="B112" s="7"/>
       <c r="C112" s="7"/>
       <c r="D112" s="7"/>
       <c r="E112" s="7"/>
     </row>
-    <row r="113" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" s="14" t="s">
         <v>137</v>
       </c>
@@ -2420,7 +2423,7 @@
       <c r="D113" s="7"/>
       <c r="E113" s="7"/>
     </row>
-    <row r="114" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>237</v>
       </c>
@@ -2434,7 +2437,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="115" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>238</v>
       </c>
@@ -2445,7 +2448,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="116" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>239</v>
       </c>
@@ -2459,7 +2462,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="117" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B117" t="s">
         <v>144</v>
       </c>
@@ -2467,12 +2470,12 @@
         <v>232</v>
       </c>
     </row>
-    <row r="118" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B118" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="119" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>240</v>
       </c>
@@ -2486,17 +2489,17 @@
         <v>233</v>
       </c>
     </row>
-    <row r="120" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B120" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="121" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B121" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="122" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" s="3" t="s">
         <v>234</v>
       </c>
@@ -2510,7 +2513,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="123" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C123" t="s">
         <v>253</v>
       </c>
@@ -2518,12 +2521,12 @@
         <v>254</v>
       </c>
     </row>
-    <row r="124" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C124" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="125" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C125" t="s">
         <v>255</v>
       </c>
@@ -2531,12 +2534,12 @@
         <v>256</v>
       </c>
     </row>
-    <row r="126" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C126" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="127" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C127" t="s">
         <v>257</v>
       </c>
@@ -2544,7 +2547,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="128" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>235</v>
       </c>
@@ -2561,7 +2564,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="129" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>236</v>
       </c>
@@ -2578,7 +2581,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="130" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C130" t="s">
         <v>262</v>
       </c>
@@ -2586,16 +2589,15 @@
         <v>263</v>
       </c>
     </row>
-    <row r="131" spans="1:5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="132" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A132" s="7"/>
     </row>
-    <row r="133" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A133" s="6" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="134" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>265</v>
       </c>
@@ -2608,6 +2610,12 @@
     <row r="136" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>267</v>
+      </c>
+      <c r="B136" t="s">
+        <v>270</v>
+      </c>
+      <c r="C136" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Lista incluye ocu. cam. hosp.
</commit_message>
<xml_diff>
--- a/Lista_programas_inputs_outputs.xlsx
+++ b/Lista_programas_inputs_outputs.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\GitHub\covid_cusco\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F2957CC-41AF-47FF-BA2D-C30F9AB56DAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{112F37C3-B048-4966-B8E9-CEE329E10364}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-13704" yWindow="8448" windowWidth="23040" windowHeight="7320" xr2:uid="{6F1C67DC-F352-4C08-898E-8C30B2794AD3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6F1C67DC-F352-4C08-898E-8C30B2794AD3}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Hoja1!$A$1:$E$140</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Hoja1!$A$1:$E$141</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="275">
   <si>
     <t>Programa</t>
   </si>
@@ -870,6 +870,18 @@
   </si>
   <si>
     <t>4z_tabla_cero_defunciones.do</t>
+  </si>
+  <si>
+    <t>base_ocupacion_camas_hospitalarias.xlsx</t>
+  </si>
+  <si>
+    <t>(Actualiza semanalmente la ocupación de camas hospitalarias)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actualizar la ocupación de camas hospitalarias en el Dashboard </t>
+  </si>
+  <si>
+    <t>C:\Users\HP\Documents\GitHub\covid-cusco\dashboard-covid-geresa\data\source1_camas\main</t>
   </si>
 </sst>
 </file>
@@ -1315,10 +1327,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:XFD138"/>
+  <dimension ref="A1:XFD139"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A108" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D137" sqref="D137"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A30" zoomScale="82" zoomScaleNormal="100" zoomScaleSheetLayoutView="82" workbookViewId="0">
+      <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1787,7 +1799,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="48" spans="1:5 16384:16384" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5 16384:16384" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A48" s="15" t="s">
         <v>132</v>
       </c>
@@ -1802,829 +1814,844 @@
         <v>212</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A50" s="5" t="s">
+    <row r="49" spans="1:5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A49" s="15" t="s">
+        <v>274</v>
+      </c>
+      <c r="B49" s="9" t="s">
+        <v>271</v>
+      </c>
+      <c r="C49" s="9" t="s">
+        <v>272</v>
+      </c>
+      <c r="D49" s="13"/>
+      <c r="E49" s="9" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="5" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
+    <row r="52" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
         <v>58</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B52" t="s">
         <v>41</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C52" t="s">
         <v>59</v>
       </c>
-      <c r="E51" t="s">
+      <c r="E52" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
+    <row r="53" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
         <v>60</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B53" t="s">
         <v>59</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C53" t="s">
         <v>61</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D53" t="s">
         <v>62</v>
       </c>
-      <c r="E52" t="s">
+      <c r="E53" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C53" t="s">
+    <row r="54" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C54" t="s">
         <v>64</v>
       </c>
-      <c r="D53" t="s">
+      <c r="D54" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C54" t="s">
+    <row r="55" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C55" t="s">
         <v>65</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D55" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C55" t="s">
+    <row r="56" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C56" t="s">
         <v>67</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D56" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C56" t="s">
+    <row r="57" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C57" t="s">
         <v>69</v>
       </c>
-      <c r="D56" t="s">
+      <c r="D57" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C57" t="s">
+    <row r="58" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C58" t="s">
         <v>71</v>
       </c>
-      <c r="D57" t="s">
+      <c r="D58" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C58" t="s">
+    <row r="59" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C59" t="s">
         <v>73</v>
       </c>
-      <c r="D58" t="s">
+      <c r="D59" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
+    <row r="60" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
         <v>75</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B60" t="s">
         <v>38</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C60" t="s">
         <v>76</v>
       </c>
-      <c r="E59" t="s">
+      <c r="E60" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C60" t="s">
+    <row r="61" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C61" t="s">
         <v>77</v>
       </c>
-      <c r="D60" t="s">
+      <c r="D61" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C61" t="s">
+    <row r="62" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C62" t="s">
         <v>78</v>
       </c>
-      <c r="D61" t="s">
+      <c r="D62" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C62" t="s">
+    <row r="63" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C63" t="s">
         <v>80</v>
       </c>
-      <c r="D62" t="s">
+      <c r="D63" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C63" t="s">
+    <row r="64" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C64" t="s">
         <v>82</v>
       </c>
-      <c r="D63" t="s">
+      <c r="D64" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C64" t="s">
+    <row r="65" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C65" t="s">
         <v>84</v>
       </c>
-      <c r="D64" t="s">
+      <c r="D65" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C65" t="s">
+    <row r="66" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C66" t="s">
         <v>86</v>
       </c>
-      <c r="D65" t="s">
+      <c r="D66" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C66" t="s">
+    <row r="67" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C67" t="s">
         <v>88</v>
       </c>
-      <c r="D66" t="s">
+      <c r="D67" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
+    <row r="68" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
         <v>90</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B68" t="s">
         <v>105</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C68" t="s">
         <v>92</v>
       </c>
-      <c r="E67" t="s">
+      <c r="E68" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A68" t="s">
+    <row r="69" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
         <v>94</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B69" t="s">
         <v>92</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C69" t="s">
         <v>95</v>
       </c>
-      <c r="D68" t="s">
+      <c r="D69" t="s">
         <v>96</v>
       </c>
-      <c r="E68" t="s">
+      <c r="E69" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C69" t="s">
+    <row r="70" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C70" t="s">
         <v>97</v>
       </c>
-      <c r="D69" t="s">
+      <c r="D70" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A70" t="s">
+    <row r="71" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
         <v>101</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B71" t="s">
         <v>93</v>
       </c>
-      <c r="C70" s="3" t="s">
+      <c r="C71" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="E70" t="s">
+      <c r="E71" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C71" t="s">
+    <row r="72" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C72" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C72" t="s">
+    <row r="73" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C73" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A73" t="s">
+    <row r="74" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
         <v>104</v>
-      </c>
-      <c r="B73" t="s">
-        <v>103</v>
-      </c>
-      <c r="C73" t="s">
-        <v>102</v>
-      </c>
-      <c r="E73" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A74" t="s">
-        <v>107</v>
       </c>
       <c r="B74" t="s">
         <v>103</v>
       </c>
       <c r="C74" t="s">
+        <v>102</v>
+      </c>
+      <c r="E74" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>107</v>
+      </c>
+      <c r="B75" t="s">
+        <v>103</v>
+      </c>
+      <c r="C75" t="s">
         <v>108</v>
       </c>
-      <c r="E74" t="s">
+      <c r="E75" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A75" t="s">
+    <row r="76" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
         <v>112</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B76" t="s">
         <v>99</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C76" t="s">
         <v>110</v>
       </c>
-      <c r="D75" t="s">
+      <c r="D76" t="s">
         <v>111</v>
       </c>
-      <c r="E75" t="s">
+      <c r="E76" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B76" t="s">
+    <row r="77" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B77" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A77" t="s">
+    <row r="78" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
         <v>113</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B78" t="s">
         <v>100</v>
       </c>
-      <c r="C77" t="s">
+      <c r="C78" t="s">
         <v>114</v>
       </c>
-      <c r="D77" t="s">
+      <c r="D78" t="s">
         <v>115</v>
       </c>
-      <c r="E77" t="s">
+      <c r="E78" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B78" t="s">
+    <row r="79" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B79" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A79" t="s">
+    <row r="80" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
         <v>123</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B80" t="s">
         <v>116</v>
       </c>
-      <c r="C79" t="s">
+      <c r="C80" t="s">
         <v>118</v>
       </c>
-      <c r="D79" t="s">
+      <c r="D80" t="s">
         <v>117</v>
       </c>
-      <c r="E79" t="s">
+      <c r="E80" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C80" t="s">
+    <row r="81" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C81" t="s">
         <v>120</v>
       </c>
-      <c r="D80" t="s">
+      <c r="D81" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C81" t="s">
+    <row r="82" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C82" t="s">
         <v>121</v>
       </c>
-      <c r="D81" t="s">
+      <c r="D82" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C82" t="s">
+    <row r="83" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C83" t="s">
         <v>125</v>
       </c>
-      <c r="D82" t="s">
+      <c r="D83" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C83" t="s">
+    <row r="84" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C84" t="s">
         <v>126</v>
       </c>
-      <c r="D83" t="s">
+      <c r="D84" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A84" s="13"/>
-      <c r="B84" s="13"/>
-      <c r="C84" s="13" t="s">
+    <row r="85" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="13"/>
+      <c r="B85" s="13"/>
+      <c r="C85" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="D84" s="13" t="s">
+      <c r="D85" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="E84" s="13"/>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A85" s="7"/>
-      <c r="B85" s="7"/>
-      <c r="C85" s="7"/>
-      <c r="D85" s="7"/>
-      <c r="E85" s="7"/>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A86" s="6" t="s">
-        <v>150</v>
-      </c>
+      <c r="E85" s="13"/>
+    </row>
+    <row r="86" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="7"/>
       <c r="B86" s="7"/>
       <c r="C86" s="7"/>
       <c r="D86" s="7"/>
       <c r="E86" s="7"/>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A87" t="s">
+    <row r="87" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="B87" s="7"/>
+      <c r="C87" s="7"/>
+      <c r="D87" s="7"/>
+      <c r="E87" s="7"/>
+    </row>
+    <row r="88" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
         <v>151</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B88" t="s">
         <v>156</v>
       </c>
-      <c r="C87" t="s">
+      <c r="C88" t="s">
         <v>165</v>
       </c>
-      <c r="E87" t="s">
+      <c r="E88" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B88" t="s">
+    <row r="89" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B89" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B89" t="s">
+    <row r="90" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B90" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B90" t="s">
+    <row r="91" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B91" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B91" t="s">
+    <row r="92" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B92" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B92" t="s">
+    <row r="93" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B93" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B93" t="s">
+    <row r="94" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B94" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A94" t="s">
+    <row r="95" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
         <v>152</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B95" t="s">
         <v>163</v>
       </c>
-      <c r="C94" t="s">
+      <c r="C95" t="s">
         <v>170</v>
       </c>
-      <c r="E94" t="s">
+      <c r="E95" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A95" t="s">
+    <row r="96" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
         <v>153</v>
       </c>
-      <c r="B95" t="s">
+      <c r="B96" t="s">
         <v>165</v>
       </c>
-      <c r="E95" t="s">
+      <c r="E96" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B96" t="s">
+    <row r="97" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B97" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A97" t="s">
+    <row r="98" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
         <v>154</v>
       </c>
-      <c r="B97" t="s">
+      <c r="B98" t="s">
         <v>170</v>
       </c>
-      <c r="C97" t="s">
+      <c r="C98" t="s">
         <v>184</v>
       </c>
-      <c r="D97" t="s">
+      <c r="D98" t="s">
         <v>185</v>
       </c>
-      <c r="E97" t="s">
+      <c r="E98" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A98" t="s">
+    <row r="99" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
         <v>155</v>
       </c>
-      <c r="B98" t="s">
+      <c r="B99" t="s">
         <v>166</v>
       </c>
-      <c r="C98" t="s">
+      <c r="C99" t="s">
         <v>172</v>
       </c>
-      <c r="D98" t="s">
+      <c r="D99" t="s">
         <v>173</v>
       </c>
-      <c r="E98" t="s">
+      <c r="E99" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B99" t="s">
+    <row r="100" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B100" t="s">
         <v>167</v>
       </c>
-      <c r="C99" t="s">
+      <c r="C100" t="s">
         <v>174</v>
       </c>
-      <c r="D99" t="s">
+      <c r="D100" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B100" t="s">
-        <v>168</v>
-      </c>
-      <c r="C100" t="s">
-        <v>176</v>
-      </c>
-      <c r="D100" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B101" t="s">
         <v>168</v>
       </c>
       <c r="C101" t="s">
+        <v>176</v>
+      </c>
+      <c r="D101" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B102" t="s">
+        <v>168</v>
+      </c>
+      <c r="C102" t="s">
         <v>178</v>
       </c>
-      <c r="D101" t="s">
+      <c r="D102" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B102" t="s">
+    <row r="103" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B103" t="s">
         <v>169</v>
       </c>
-      <c r="C102" t="s">
+      <c r="C103" t="s">
         <v>180</v>
       </c>
-      <c r="D102" t="s">
+      <c r="D103" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B103" t="s">
+    <row r="104" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B104" t="s">
         <v>170</v>
       </c>
-      <c r="C103" t="s">
+      <c r="C104" t="s">
         <v>182</v>
       </c>
-      <c r="D103" t="s">
+      <c r="D104" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B104" t="s">
+    <row r="105" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B105" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A105" s="13"/>
-      <c r="B105" s="13" t="s">
+    <row r="106" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A106" s="13"/>
+      <c r="B106" s="13" t="s">
         <v>171</v>
       </c>
-      <c r="C105" s="13"/>
-      <c r="D105" s="13"/>
-      <c r="E105" s="13"/>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A106" s="7"/>
-      <c r="B106" s="7"/>
-      <c r="C106" s="7"/>
-      <c r="D106" s="7"/>
-      <c r="E106" s="7"/>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A107" s="6" t="s">
-        <v>249</v>
-      </c>
+      <c r="C106" s="13"/>
+      <c r="D106" s="13"/>
+      <c r="E106" s="13"/>
+    </row>
+    <row r="107" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A107" s="7"/>
       <c r="B107" s="7"/>
       <c r="C107" s="7"/>
       <c r="D107" s="7"/>
       <c r="E107" s="7"/>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A108" t="s">
+    <row r="108" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A108" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="B108" s="7"/>
+      <c r="C108" s="7"/>
+      <c r="D108" s="7"/>
+      <c r="E108" s="7"/>
+    </row>
+    <row r="109" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
         <v>147</v>
       </c>
-      <c r="B108" t="s">
+      <c r="B109" t="s">
         <v>148</v>
       </c>
-      <c r="C108" t="s">
+      <c r="C109" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A109" t="s">
+    <row r="110" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
         <v>186</v>
       </c>
-      <c r="B109" t="s">
-        <v>149</v>
-      </c>
-      <c r="C109" t="s">
-        <v>187</v>
-      </c>
-      <c r="D109" t="s">
-        <v>188</v>
-      </c>
-      <c r="E109" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B110" t="s">
         <v>149</v>
       </c>
       <c r="C110" t="s">
+        <v>187</v>
+      </c>
+      <c r="D110" t="s">
+        <v>188</v>
+      </c>
+      <c r="E110" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B111" t="s">
+        <v>149</v>
+      </c>
+      <c r="C111" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B111" t="s">
+    <row r="112" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B112" t="s">
         <v>6</v>
       </c>
-      <c r="C111" t="s">
+      <c r="C112" t="s">
         <v>190</v>
       </c>
-      <c r="D111" t="s">
+      <c r="D112" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A112" s="7"/>
-      <c r="B112" s="7"/>
-      <c r="C112" s="7"/>
-      <c r="D112" s="7"/>
-      <c r="E112" s="7"/>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A113" s="14" t="s">
-        <v>137</v>
-      </c>
+    <row r="113" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A113" s="7"/>
       <c r="B113" s="7"/>
       <c r="C113" s="7"/>
       <c r="D113" s="7"/>
       <c r="E113" s="7"/>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A114" t="s">
+    <row r="114" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A114" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="B114" s="7"/>
+      <c r="C114" s="7"/>
+      <c r="D114" s="7"/>
+      <c r="E114" s="7"/>
+    </row>
+    <row r="115" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
         <v>237</v>
       </c>
-      <c r="B114" s="2" t="s">
+      <c r="B115" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="C114" t="s">
+      <c r="C115" t="s">
         <v>141</v>
-      </c>
-      <c r="E114" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A115" t="s">
-        <v>238</v>
-      </c>
-      <c r="B115" t="s">
-        <v>10</v>
       </c>
       <c r="E115" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
+        <v>238</v>
+      </c>
+      <c r="B116" t="s">
+        <v>10</v>
+      </c>
+      <c r="E116" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
         <v>239</v>
       </c>
-      <c r="B116" t="s">
+      <c r="B117" t="s">
         <v>143</v>
       </c>
-      <c r="C116" t="s">
+      <c r="C117" t="s">
         <v>145</v>
       </c>
-      <c r="E116" t="s">
+      <c r="E117" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B117" t="s">
+    <row r="118" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B118" t="s">
         <v>144</v>
       </c>
-      <c r="E117" t="s">
+      <c r="E118" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B118" t="s">
+    <row r="119" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B119" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A119" t="s">
+    <row r="120" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
         <v>240</v>
       </c>
-      <c r="B119" t="s">
+      <c r="B120" t="s">
         <v>141</v>
       </c>
-      <c r="C119" t="s">
+      <c r="C120" t="s">
         <v>146</v>
       </c>
-      <c r="E119" t="s">
+      <c r="E120" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B120" t="s">
+    <row r="121" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B121" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B121" t="s">
+    <row r="122" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B122" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A122" s="3" t="s">
+    <row r="123" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A123" s="3" t="s">
         <v>234</v>
       </c>
-      <c r="B122" t="s">
+      <c r="B123" t="s">
         <v>146</v>
       </c>
-      <c r="C122" t="s">
+      <c r="C123" t="s">
         <v>241</v>
       </c>
-      <c r="E122" t="s">
+      <c r="E123" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C123" t="s">
+    <row r="124" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C124" t="s">
         <v>253</v>
       </c>
-      <c r="D123" t="s">
+      <c r="D124" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C124" t="s">
+    <row r="125" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C125" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C125" t="s">
+    <row r="126" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C126" t="s">
         <v>255</v>
       </c>
-      <c r="D125" t="s">
+      <c r="D126" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C126" t="s">
+    <row r="127" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C127" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C127" t="s">
+    <row r="128" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C128" t="s">
         <v>257</v>
       </c>
-      <c r="D127" t="s">
+      <c r="D128" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A128" t="s">
+    <row r="129" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
         <v>235</v>
       </c>
-      <c r="B128" t="s">
+      <c r="B129" t="s">
         <v>32</v>
       </c>
-      <c r="C128" t="s">
+      <c r="C129" t="s">
         <v>260</v>
       </c>
-      <c r="D128" t="s">
+      <c r="D129" t="s">
         <v>261</v>
       </c>
-      <c r="E128" t="s">
+      <c r="E129" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A129" t="s">
+    <row r="130" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A130" t="s">
         <v>236</v>
       </c>
-      <c r="B129" t="s">
+      <c r="B130" t="s">
         <v>44</v>
       </c>
-      <c r="C129" t="s">
+      <c r="C130" t="s">
         <v>244</v>
       </c>
-      <c r="D129" t="s">
+      <c r="D130" t="s">
         <v>245</v>
       </c>
-      <c r="E129" t="s">
+      <c r="E130" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C130" t="s">
+    <row r="131" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C131" t="s">
         <v>262</v>
       </c>
-      <c r="D130" t="s">
+      <c r="D131" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A132" s="7"/>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A133" s="6" t="s">
+    <row r="133" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A133" s="7"/>
+    </row>
+    <row r="134" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A134" s="6" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A134" t="s">
+    <row r="135" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A135" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A135" t="s">
+    <row r="136" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A136" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A136" t="s">
+    <row r="137" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A137" t="s">
         <v>267</v>
       </c>
-      <c r="B136" t="s">
+      <c r="B137" t="s">
         <v>270</v>
       </c>
-      <c r="C136" t="s">
+      <c r="C137" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A137" t="s">
+    <row r="138" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A138" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A138" t="s">
+    <row r="139" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A139" t="s">
         <v>269</v>
       </c>
     </row>
@@ -2633,7 +2660,7 @@
   <pageSetup scale="50" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <rowBreaks count="2" manualBreakCount="2">
     <brk id="44" max="16383" man="1"/>
-    <brk id="84" max="16383" man="1"/>
+    <brk id="85" max="16383" man="1"/>
   </rowBreaks>
 </worksheet>
 </file>
</xml_diff>